<commit_message>
add style, back link, description
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nikol\source\repos\esveske\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5088EDE-2DEC-4BAA-B245-4BDC877D383B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D75CA94-8AD2-45E3-8EFB-6A6148ABA601}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{635E8188-4706-48C9-A343-ED53CEC08EDF}"/>
   </bookViews>
@@ -13842,8 +13842,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:K1892"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1670" workbookViewId="0">
-      <selection activeCell="A1691" sqref="A1691"/>
+    <sheetView tabSelected="1" topLeftCell="A1673" workbookViewId="0">
+      <selection activeCell="J1684" sqref="J1684"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
update data because .pdf missing
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -14794,7 +14794,7 @@
     <t xml:space="preserve">Intersubjektivnost i telesno iskustvo u praksama čitanja tarota</t>
   </si>
   <si>
-    <t xml:space="preserve">pdf/2019/PS78-Zb2019_III-ANT-MB</t>
+    <t xml:space="preserve">pdf/2019/PS78-Zb2019_III-ANT-MB.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Lazarević Mateja </t>
@@ -14806,7 +14806,7 @@
     <t xml:space="preserve">Narativi i prakse solidarnosti u kontekstu borbe protiv deložacija</t>
   </si>
   <si>
-    <t xml:space="preserve">pdf/2019/PS78-Zb2019_III-ANT-ML</t>
+    <t xml:space="preserve">pdf/2019/PS78-Zb2019_III-ANT-ML.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Kačar Atina </t>
@@ -14818,7 +14818,7 @@
     <t xml:space="preserve">Šta znači biti dobar roditelj? Narativi o roditeljstvu u peroiodu neoliberalizma</t>
   </si>
   <si>
-    <t xml:space="preserve">pdf/2019/PS78-Zb2019_III-ANT-AKLT</t>
+    <t xml:space="preserve">pdf/2019/PS78-Zb2019_III-ANT-AKLT.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Trifunović Lena</t>
@@ -14830,7 +14830,7 @@
     <t xml:space="preserve">Stilska i hemijska analiza prestonih ikona ikonostasa crkve Uspenja Presvete Bogorodice u Petnici</t>
   </si>
   <si>
-    <t xml:space="preserve">pdf/2019/PS78-Zb2019_III-AHL-MMNP</t>
+    <t xml:space="preserve">pdf/2019/PS78-Zb2019_III-AHL-MMNP.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Nježić Teodora</t>
@@ -14842,13 +14842,13 @@
     <t xml:space="preserve">Analiza ugljenisanih ostataka drveta iz objekata 1 i 2 sa lokaliteta Anine u Ćelijama</t>
   </si>
   <si>
-    <t xml:space="preserve">pdf/2019/PS78-Zb2019_III-AHL-TN</t>
+    <t xml:space="preserve">pdf/2019/PS78-Zb2019_III-AHL-TN.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Predstave evharistijskih posuda na liturgijskim scenama u doba Renesanse Paleologa u hramovima srpskih ktitora</t>
   </si>
   <si>
-    <t xml:space="preserve">pdf/2019/PS78-Zb2019_III-AHL-MS</t>
+    <t xml:space="preserve">pdf/2019/PS78-Zb2019_III-AHL-MS.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Trajković Katarina</t>
@@ -14860,7 +14860,7 @@
     <t xml:space="preserve">Analiza skeletnih ostataka iz grobova 112, 114 i 123 sa lokaliteta Slavkovica</t>
   </si>
   <si>
-    <t xml:space="preserve">pdf/2019/PS78-Zb2019_III-AHL-KT</t>
+    <t xml:space="preserve">pdf/2019/PS78-Zb2019_III-AHL-KT.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Đorđević Mina</t>
@@ -14872,7 +14872,7 @@
     <t xml:space="preserve">Rezervisano: mladi o ambijentima koncerata klasične muzike</t>
   </si>
   <si>
-    <t xml:space="preserve">pdf/2019/PS78-Zb2019_III-DHN-MDj</t>
+    <t xml:space="preserve">pdf/2019/PS78-Zb2019_III-DHN-MDj.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Radić Kiša</t>
@@ -14884,7 +14884,7 @@
     <t xml:space="preserve">Motivacija za izradu kognitivnih zadataka - uloga samopouzdanja i muzike</t>
   </si>
   <si>
-    <t xml:space="preserve">pdf/2019/PS78-Zb2019_III-DHN-KR</t>
+    <t xml:space="preserve">pdf/2019/PS78-Zb2019_III-DHN-KR.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Nojić Lena</t>
@@ -14893,7 +14893,7 @@
     <t xml:space="preserve">Autobiografska sećanja na detinjstvo: Šta čini sećanja upečatljivim</t>
   </si>
   <si>
-    <t xml:space="preserve">pdf/2019/PS78-Zb2019_III-DHN-LN</t>
+    <t xml:space="preserve">pdf/2019/PS78-Zb2019_III-DHN-LN.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Babić Milica</t>
@@ -14905,13 +14905,13 @@
     <t xml:space="preserve">Očekivanje dece predškolskog uzrasta o početku prvog razreda</t>
   </si>
   <si>
-    <t xml:space="preserve">pdf/2019/PS78-Zb2019_III-DHN-MB</t>
+    <t xml:space="preserve">pdf/2019/PS78-Zb2019_III-DHN-MB.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Sreski odbor Saveza ratnih vojnih invalida u Valjevu (1950 - 1962)</t>
   </si>
   <si>
-    <t xml:space="preserve">pdf/2019/PS78-Zb2019_III-IST-PI</t>
+    <t xml:space="preserve">pdf/2019/PS78-Zb2019_III-IST-PI.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Milekovič Ivan</t>
@@ -14920,7 +14920,7 @@
     <t xml:space="preserve">Jugoslovenstvo u slobodnozidarskim ložama Beograda i Zagreba</t>
   </si>
   <si>
-    <t xml:space="preserve">pdf/2019/PS78-Zb2019_III-IST-IM</t>
+    <t xml:space="preserve">pdf/2019/PS78-Zb2019_III-IST-IM.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Žunić Konstantin</t>
@@ -14929,7 +14929,7 @@
     <t xml:space="preserve">Odnos vlasti i Udruženja Južnosrbijanaca 1929-1943</t>
   </si>
   <si>
-    <t xml:space="preserve">pdf/2019/PS78-Zb2019_III-IST-KZh</t>
+    <t xml:space="preserve">pdf/2019/PS78-Zb2019_III-IST-KZh.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Ekonomska škola "Đuka Dinić"</t>
@@ -14938,7 +14938,7 @@
     <t xml:space="preserve">Integrisanje Banjalučkog okruga u politički i ekonomski sistem Kraljevine SHS</t>
   </si>
   <si>
-    <t xml:space="preserve">pdf/2019/PS78-Zb2019_III-IST-MM</t>
+    <t xml:space="preserve">pdf/2019/PS78-Zb2019_III-IST-MM.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Samočeta Jelena</t>
@@ -14947,7 +14947,7 @@
     <t xml:space="preserve">Tipovi metonimije u nazivima za psihoaktivne supstance u slengu</t>
   </si>
   <si>
-    <t xml:space="preserve">pdf/2019/PS78-Zb2019_III-LIN-JS</t>
+    <t xml:space="preserve">pdf/2019/PS78-Zb2019_III-LIN-JS.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Savić Helena</t>
@@ -14956,7 +14956,7 @@
     <t xml:space="preserve">Stavovi mađarsko-srpskih bilingvala prema srpskom jeziku</t>
   </si>
   <si>
-    <t xml:space="preserve">pdf/2019/PS78-Zb2019_III-LIN-HS</t>
+    <t xml:space="preserve">pdf/2019/PS78-Zb2019_III-LIN-HS.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Despotović Nela</t>
@@ -14968,7 +14968,7 @@
     <t xml:space="preserve">Rod u jezicu: Antropolingvistički pogled na stanje u italijanskom i danskom jeziku</t>
   </si>
   <si>
-    <t xml:space="preserve">pdf/2019/PS78-Zb2019_III-LIN-ND</t>
+    <t xml:space="preserve">pdf/2019/PS78-Zb2019_III-LIN-ND.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Savić Katarina</t>
@@ -14977,7 +14977,7 @@
     <t xml:space="preserve">Komparativna analiza frazeologizama sa nazivima domaćih životnja u srpskom i italijanskom jeziku</t>
   </si>
   <si>
-    <t xml:space="preserve">pdf/2019/PS78-Zb2019_III-LIN-KS</t>
+    <t xml:space="preserve">pdf/2019/PS78-Zb2019_III-LIN-KS.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Sakule</t>
@@ -14986,7 +14986,7 @@
     <t xml:space="preserve">Efekat homogenog grupisanja i lingvističke darovitosti na lingvistički self-koncept i jezičku anksioznost srednjoškolaca</t>
   </si>
   <si>
-    <t xml:space="preserve">pdf/2019/PS78-Zb2019_III-PSI-DO</t>
+    <t xml:space="preserve">pdf/2019/PS78-Zb2019_III-PSI-DO.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Zubnar Dušan</t>
@@ -14995,7 +14995,7 @@
     <t xml:space="preserve">Predviđanje konzervativnosti stava načinima prevazilaženja stresa pri odlučivanju</t>
   </si>
   <si>
-    <t xml:space="preserve">pdf/2019/PS78-Zb2019_III-PSI-DZVP</t>
+    <t xml:space="preserve">pdf/2019/PS78-Zb2019_III-PSI-DZVP.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Plavšić Vladana</t>
@@ -15007,7 +15007,7 @@
     <t xml:space="preserve">Uticaj auditivnog primovanja u vizelnoj pretrazi u normalnim i degradiranim uslovima</t>
   </si>
   <si>
-    <t xml:space="preserve">pdf/2019/PS78-Zb2019_III-PSI-VJ</t>
+    <t xml:space="preserve">pdf/2019/PS78-Zb2019_III-PSI-VJ.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Crnogorac Mina</t>
@@ -15016,7 +15016,7 @@
     <t xml:space="preserve">Odnos adolescenata Srbije prema generički modifikovanoj hrani: uverenja, objektivno i samoprocenjeno znanje</t>
   </si>
   <si>
-    <t xml:space="preserve">pdf/2019/PS78-Zb2019_III-PSI-MC</t>
+    <t xml:space="preserve">pdf/2019/PS78-Zb2019_III-PSI-MC.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Matevska Mina</t>
@@ -15025,7 +15025,7 @@
     <t xml:space="preserve">Srednja turistička škola</t>
   </si>
   <si>
-    <t xml:space="preserve">pdf/2019/PS78-Zb2019_III-PSI-MM</t>
+    <t xml:space="preserve">pdf/2019/PS78-Zb2019_III-PSI-MM.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Seminar dizajna 2019</t>
@@ -15165,11 +15165,11 @@
   </sheetPr>
   <dimension ref="A1:L2126"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2012" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2033" activeCellId="0" sqref="E2033"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K2083" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N2116" activeCellId="0" sqref="N2116"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.14"/>
@@ -77715,7 +77715,7 @@
         <v>13</v>
       </c>
       <c r="G2089" s="3" t="s">
-        <v>4885</v>
+        <v>114</v>
       </c>
       <c r="H2089" s="1"/>
       <c r="I2089" s="3" t="n">
@@ -77748,7 +77748,7 @@
         <v>13</v>
       </c>
       <c r="G2090" s="3" t="s">
-        <v>4885</v>
+        <v>114</v>
       </c>
       <c r="H2090" s="1"/>
       <c r="I2090" s="3" t="n">
@@ -77781,7 +77781,7 @@
         <v>2350</v>
       </c>
       <c r="G2091" s="3" t="s">
-        <v>4885</v>
+        <v>114</v>
       </c>
       <c r="H2091" s="1"/>
       <c r="I2091" s="3" t="n">
@@ -77814,7 +77814,7 @@
         <v>21</v>
       </c>
       <c r="G2092" s="3" t="s">
-        <v>4885</v>
+        <v>114</v>
       </c>
       <c r="H2092" s="1"/>
       <c r="I2092" s="3" t="n">
@@ -77847,7 +77847,7 @@
         <v>13</v>
       </c>
       <c r="G2093" s="3" t="s">
-        <v>4885</v>
+        <v>114</v>
       </c>
       <c r="H2093" s="1"/>
       <c r="I2093" s="3" t="n">
@@ -77880,7 +77880,7 @@
         <v>853</v>
       </c>
       <c r="G2094" s="3" t="s">
-        <v>4885</v>
+        <v>114</v>
       </c>
       <c r="H2094" s="1"/>
       <c r="I2094" s="3" t="n">

</xml_diff>